<commit_message>
added MolProbity scores for CEP290, DHDDS, GUCA1A, GUCY2D, IQCB1 and updated VVD-structures-results.xlsx
</commit_message>
<xml_diff>
--- a/VVD-structures-results.xlsx
+++ b/VVD-structures-results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="22840" yWindow="0" windowWidth="21580" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="21100" yWindow="40" windowWidth="14200" windowHeight="19420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -448,8 +448,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -554,19 +556,19 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -578,11 +580,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -614,6 +616,7 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -645,6 +648,7 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -976,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1036,10 +1040,10 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="3">
@@ -1065,8 +1069,8 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
         <v>11</v>
@@ -1088,8 +1092,8 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="4">
@@ -1115,8 +1119,8 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
         <v>11</v>
@@ -1138,8 +1142,8 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="4">
@@ -1188,10 +1192,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" s="11" customFormat="1">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="15" t="s">
         <v>98</v>
       </c>
       <c r="C9" s="9"/>
@@ -1215,8 +1219,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" s="11" customFormat="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9" t="s">
         <v>11</v>
@@ -1228,8 +1232,8 @@
       <c r="I10" s="9"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17" t="s">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="1">
@@ -1256,7 +1260,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="16"/>
-      <c r="B12" s="17"/>
+      <c r="B12" s="18"/>
       <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1277,10 +1281,10 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="3"/>
@@ -1327,10 +1331,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" s="11" customFormat="1">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="15" t="s">
         <v>85</v>
       </c>
       <c r="C15" s="9"/>
@@ -1377,10 +1381,10 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="8">
@@ -1407,7 +1411,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="16"/>
-      <c r="B18" s="15"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9" t="s">
         <v>11</v>
@@ -1429,10 +1433,10 @@
       </c>
     </row>
     <row r="19" spans="1:9" s="11" customFormat="1">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>89</v>
       </c>
       <c r="C19" s="8"/>
@@ -1456,23 +1460,33 @@
       </c>
     </row>
     <row r="20" spans="1:9" s="11" customFormat="1">
-      <c r="A20" s="15"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="16"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
+      <c r="E20" s="10">
+        <v>1.8</v>
+      </c>
+      <c r="F20" s="10">
+        <v>99</v>
+      </c>
+      <c r="G20" s="10">
+        <v>5.81</v>
+      </c>
+      <c r="H20" s="10">
+        <v>2.04</v>
+      </c>
+      <c r="I20" s="10">
+        <v>74</v>
+      </c>
     </row>
     <row r="21" spans="1:9" s="11" customFormat="1">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="15" t="s">
         <v>88</v>
       </c>
       <c r="C21" s="9"/>
@@ -1502,17 +1516,12 @@
       <c r="D22" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="3"/>
@@ -1559,10 +1568,10 @@
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="18" t="s">
         <v>25</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1585,8 +1594,8 @@
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="15"/>
-      <c r="B26" s="17"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="18"/>
       <c r="D26" s="1" t="s">
         <v>11</v>
       </c>
@@ -1607,8 +1616,8 @@
       </c>
     </row>
     <row r="27" spans="1:9" s="11" customFormat="1">
-      <c r="A27" s="15"/>
-      <c r="B27" s="17" t="s">
+      <c r="A27" s="17"/>
+      <c r="B27" s="18" t="s">
         <v>99</v>
       </c>
       <c r="D27" s="11" t="s">
@@ -1638,10 +1647,10 @@
       </c>
     </row>
     <row r="29" spans="1:9" s="11" customFormat="1">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="15" t="s">
         <v>91</v>
       </c>
       <c r="C29" s="8"/>
@@ -1688,10 +1697,10 @@
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C31" s="3">
@@ -1717,8 +1726,8 @@
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
         <v>11</v>
@@ -1740,8 +1749,8 @@
       </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15" t="s">
+      <c r="A33" s="17"/>
+      <c r="B33" s="17" t="s">
         <v>28</v>
       </c>
       <c r="C33" s="4">
@@ -1767,8 +1776,8 @@
       </c>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4" t="s">
         <v>11</v>
@@ -1790,8 +1799,8 @@
       </c>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15" t="s">
+      <c r="A35" s="17"/>
+      <c r="B35" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C35" s="4">
@@ -1817,8 +1826,8 @@
       </c>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4" t="s">
         <v>11</v>
@@ -1840,8 +1849,8 @@
       </c>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15" t="s">
+      <c r="A37" s="17"/>
+      <c r="B37" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C37" s="4">
@@ -1867,8 +1876,8 @@
       </c>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
         <v>11</v>
@@ -1890,8 +1899,8 @@
       </c>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15" t="s">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="4">
@@ -1917,8 +1926,8 @@
       </c>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
         <v>11</v>
@@ -1940,8 +1949,8 @@
       </c>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15" t="s">
+      <c r="A41" s="17"/>
+      <c r="B41" s="17" t="s">
         <v>32</v>
       </c>
       <c r="C41" s="4">
@@ -1967,8 +1976,8 @@
       </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="15"/>
-      <c r="B42" s="15"/>
+      <c r="A42" s="17"/>
+      <c r="B42" s="17"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4" t="s">
         <v>11</v>
@@ -1990,8 +1999,8 @@
       </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="15"/>
-      <c r="B43" s="15" t="s">
+      <c r="A43" s="17"/>
+      <c r="B43" s="17" t="s">
         <v>33</v>
       </c>
       <c r="C43" s="4">
@@ -2017,8 +2026,8 @@
       </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="15"/>
-      <c r="B44" s="15"/>
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4" t="s">
         <v>11</v>
@@ -2040,8 +2049,8 @@
       </c>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="15"/>
-      <c r="B45" s="15" t="s">
+      <c r="A45" s="17"/>
+      <c r="B45" s="17" t="s">
         <v>34</v>
       </c>
       <c r="C45" s="4">
@@ -2067,8 +2076,8 @@
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="15"/>
-      <c r="B46" s="15"/>
+      <c r="A46" s="17"/>
+      <c r="B46" s="17"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4" t="s">
         <v>11</v>
@@ -2090,8 +2099,8 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="15"/>
-      <c r="B47" s="15" t="s">
+      <c r="A47" s="17"/>
+      <c r="B47" s="17" t="s">
         <v>35</v>
       </c>
       <c r="C47" s="4">
@@ -2117,8 +2126,8 @@
       </c>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="15"/>
-      <c r="B48" s="15"/>
+      <c r="A48" s="17"/>
+      <c r="B48" s="17"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4" t="s">
         <v>11</v>
@@ -2140,8 +2149,8 @@
       </c>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="15"/>
-      <c r="B49" s="15" t="s">
+      <c r="A49" s="17"/>
+      <c r="B49" s="17" t="s">
         <v>36</v>
       </c>
       <c r="C49" s="4">
@@ -2167,8 +2176,8 @@
       </c>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="15"/>
-      <c r="B50" s="15"/>
+      <c r="A50" s="17"/>
+      <c r="B50" s="17"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4" t="s">
         <v>11</v>
@@ -2190,8 +2199,8 @@
       </c>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="15"/>
-      <c r="B51" s="15" t="s">
+      <c r="A51" s="17"/>
+      <c r="B51" s="17" t="s">
         <v>37</v>
       </c>
       <c r="C51" s="4">
@@ -2240,10 +2249,10 @@
       </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="17" t="s">
+      <c r="A53" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="18" t="s">
         <v>39</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -2266,8 +2275,8 @@
       </c>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="17"/>
-      <c r="B54" s="17"/>
+      <c r="A54" s="18"/>
+      <c r="B54" s="18"/>
       <c r="D54" s="1" t="s">
         <v>11</v>
       </c>
@@ -2288,10 +2297,10 @@
       </c>
     </row>
     <row r="55" spans="1:9" s="11" customFormat="1">
-      <c r="A55" s="14" t="s">
+      <c r="A55" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="15" t="s">
         <v>101</v>
       </c>
       <c r="C55" s="8"/>
@@ -2321,17 +2330,27 @@
       <c r="D56" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
-      <c r="H56" s="10"/>
-      <c r="I56" s="10"/>
+      <c r="E56" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="F56" s="10">
+        <v>99</v>
+      </c>
+      <c r="G56" s="10">
+        <v>14.15</v>
+      </c>
+      <c r="H56" s="10">
+        <v>2.21</v>
+      </c>
+      <c r="I56" s="10">
+        <v>64</v>
+      </c>
     </row>
     <row r="57" spans="1:9" s="11" customFormat="1">
-      <c r="A57" s="14" t="s">
+      <c r="A57" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="15" t="s">
         <v>103</v>
       </c>
       <c r="C57" s="9"/>
@@ -2355,8 +2374,8 @@
       </c>
     </row>
     <row r="58" spans="1:9" s="11" customFormat="1">
-      <c r="A58" s="15"/>
-      <c r="B58" s="15"/>
+      <c r="A58" s="17"/>
+      <c r="B58" s="17"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9" t="s">
         <v>11</v>
@@ -2368,10 +2387,10 @@
       <c r="I58" s="9"/>
     </row>
     <row r="59" spans="1:9" s="11" customFormat="1">
-      <c r="A59" s="14" t="s">
+      <c r="A59" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="15" t="s">
         <v>105</v>
       </c>
       <c r="C59" s="8"/>
@@ -2395,23 +2414,33 @@
       </c>
     </row>
     <row r="60" spans="1:9" s="11" customFormat="1">
-      <c r="A60" s="15"/>
-      <c r="B60" s="15"/>
+      <c r="A60" s="17"/>
+      <c r="B60" s="17"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="10"/>
-      <c r="H60" s="10"/>
-      <c r="I60" s="10"/>
+      <c r="E60" s="10">
+        <v>0.34</v>
+      </c>
+      <c r="F60" s="10">
+        <v>99</v>
+      </c>
+      <c r="G60" s="10">
+        <v>8.98</v>
+      </c>
+      <c r="H60" s="10">
+        <v>1.96</v>
+      </c>
+      <c r="I60" s="10">
+        <v>78</v>
+      </c>
     </row>
     <row r="61" spans="1:9" s="11" customFormat="1">
-      <c r="A61" s="14" t="s">
+      <c r="A61" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="15" t="s">
         <v>107</v>
       </c>
       <c r="C61" s="8"/>
@@ -2435,8 +2464,8 @@
       </c>
     </row>
     <row r="62" spans="1:9" s="11" customFormat="1">
-      <c r="A62" s="15"/>
-      <c r="B62" s="15"/>
+      <c r="A62" s="17"/>
+      <c r="B62" s="17"/>
       <c r="C62" s="9"/>
       <c r="D62" s="9" t="s">
         <v>11</v>
@@ -2448,8 +2477,8 @@
       <c r="I62" s="9"/>
     </row>
     <row r="63" spans="1:9" s="11" customFormat="1">
-      <c r="A63" s="15"/>
-      <c r="B63" s="15" t="s">
+      <c r="A63" s="17"/>
+      <c r="B63" s="17" t="s">
         <v>108</v>
       </c>
       <c r="C63" s="9"/>
@@ -2479,17 +2508,27 @@
       <c r="D64" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-      <c r="H64" s="9"/>
-      <c r="I64" s="9"/>
+      <c r="E64" s="9">
+        <v>0.74</v>
+      </c>
+      <c r="F64" s="9">
+        <v>99</v>
+      </c>
+      <c r="G64" s="9">
+        <v>6.04</v>
+      </c>
+      <c r="H64" s="9">
+        <v>1.9</v>
+      </c>
+      <c r="I64" s="9">
+        <v>81</v>
+      </c>
     </row>
     <row r="65" spans="1:9">
-      <c r="A65" s="14" t="s">
+      <c r="A65" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="15" t="s">
         <v>41</v>
       </c>
       <c r="C65" s="3"/>
@@ -2513,8 +2552,8 @@
       </c>
     </row>
     <row r="66" spans="1:9">
-      <c r="A66" s="15"/>
-      <c r="B66" s="15"/>
+      <c r="A66" s="17"/>
+      <c r="B66" s="17"/>
       <c r="C66" s="9"/>
       <c r="D66" s="9" t="s">
         <v>11</v>
@@ -2536,8 +2575,8 @@
       </c>
     </row>
     <row r="67" spans="1:9" s="11" customFormat="1">
-      <c r="A67" s="15"/>
-      <c r="B67" s="15" t="s">
+      <c r="A67" s="17"/>
+      <c r="B67" s="17" t="s">
         <v>109</v>
       </c>
       <c r="C67" s="9"/>
@@ -2550,7 +2589,7 @@
       <c r="F67" s="9">
         <v>0</v>
       </c>
-      <c r="G67" s="22">
+      <c r="G67" s="14">
         <v>2.94</v>
       </c>
       <c r="H67" s="9">
@@ -2567,17 +2606,27 @@
       <c r="D68" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
-      <c r="I68" s="9"/>
+      <c r="E68" s="9">
+        <v>4.24</v>
+      </c>
+      <c r="F68" s="9">
+        <v>96</v>
+      </c>
+      <c r="G68" s="9">
+        <v>4.12</v>
+      </c>
+      <c r="H68" s="9">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="I68" s="9">
+        <v>63</v>
+      </c>
     </row>
     <row r="69" spans="1:9" s="11" customFormat="1">
-      <c r="A69" s="14" t="s">
+      <c r="A69" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="15" t="s">
         <v>93</v>
       </c>
       <c r="C69" s="8"/>
@@ -2607,17 +2656,27 @@
       <c r="D70" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E70" s="10"/>
-      <c r="F70" s="10"/>
-      <c r="G70" s="10"/>
-      <c r="H70" s="10"/>
-      <c r="I70" s="10"/>
+      <c r="E70" s="10">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F70" s="10">
+        <v>99</v>
+      </c>
+      <c r="G70" s="10">
+        <v>4.04</v>
+      </c>
+      <c r="H70" s="10">
+        <v>1.41</v>
+      </c>
+      <c r="I70" s="10">
+        <v>97</v>
+      </c>
     </row>
     <row r="71" spans="1:9">
-      <c r="A71" s="17" t="s">
+      <c r="A71" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="17" t="s">
+      <c r="B71" s="18" t="s">
         <v>43</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -2640,8 +2699,8 @@
       </c>
     </row>
     <row r="72" spans="1:9">
-      <c r="A72" s="17"/>
-      <c r="B72" s="17"/>
+      <c r="A72" s="18"/>
+      <c r="B72" s="18"/>
       <c r="D72" s="1" t="s">
         <v>11</v>
       </c>
@@ -2662,10 +2721,10 @@
       </c>
     </row>
     <row r="73" spans="1:9" s="11" customFormat="1">
-      <c r="A73" s="14" t="s">
+      <c r="A73" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B73" s="15" t="s">
         <v>95</v>
       </c>
       <c r="C73" s="8"/>
@@ -2712,10 +2771,10 @@
       </c>
     </row>
     <row r="75" spans="1:9" s="11" customFormat="1">
-      <c r="A75" s="14" t="s">
+      <c r="A75" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B75" s="14" t="s">
+      <c r="B75" s="15" t="s">
         <v>97</v>
       </c>
       <c r="C75" s="9"/>
@@ -2752,10 +2811,10 @@
       <c r="I76" s="9"/>
     </row>
     <row r="77" spans="1:9">
-      <c r="A77" s="14" t="s">
+      <c r="A77" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B77" s="15" t="s">
         <v>44</v>
       </c>
       <c r="C77" s="3"/>
@@ -2802,10 +2861,10 @@
       </c>
     </row>
     <row r="79" spans="1:9">
-      <c r="A79" s="17" t="s">
+      <c r="A79" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B79" s="17" t="s">
+      <c r="B79" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -2828,8 +2887,8 @@
       </c>
     </row>
     <row r="80" spans="1:9">
-      <c r="A80" s="17"/>
-      <c r="B80" s="17"/>
+      <c r="A80" s="18"/>
+      <c r="B80" s="18"/>
       <c r="D80" s="1" t="s">
         <v>11</v>
       </c>
@@ -2850,10 +2909,10 @@
       </c>
     </row>
     <row r="81" spans="1:9">
-      <c r="A81" s="14" t="s">
+      <c r="A81" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B81" s="14" t="s">
+      <c r="B81" s="15" t="s">
         <v>49</v>
       </c>
       <c r="C81" s="3"/>
@@ -2877,8 +2936,8 @@
       </c>
     </row>
     <row r="82" spans="1:9">
-      <c r="A82" s="15"/>
-      <c r="B82" s="15"/>
+      <c r="A82" s="17"/>
+      <c r="B82" s="17"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4" t="s">
         <v>11</v>
@@ -2900,8 +2959,8 @@
       </c>
     </row>
     <row r="83" spans="1:9">
-      <c r="A83" s="15"/>
-      <c r="B83" s="15" t="s">
+      <c r="A83" s="17"/>
+      <c r="B83" s="17" t="s">
         <v>48</v>
       </c>
       <c r="C83" s="4"/>
@@ -2948,10 +3007,10 @@
       </c>
     </row>
     <row r="85" spans="1:9">
-      <c r="A85" s="14" t="s">
+      <c r="A85" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B85" s="14" t="s">
+      <c r="B85" s="15" t="s">
         <v>51</v>
       </c>
       <c r="D85" s="1" t="s">
@@ -2996,10 +3055,10 @@
       </c>
     </row>
     <row r="87" spans="1:9">
-      <c r="A87" s="14" t="s">
+      <c r="A87" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B87" s="14" t="s">
+      <c r="B87" s="15" t="s">
         <v>53</v>
       </c>
       <c r="C87" s="3"/>
@@ -3046,10 +3105,10 @@
       </c>
     </row>
     <row r="89" spans="1:9">
-      <c r="A89" s="17" t="s">
+      <c r="A89" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B89" s="17" t="s">
+      <c r="B89" s="18" t="s">
         <v>55</v>
       </c>
       <c r="D89" s="1" t="s">
@@ -3072,8 +3131,8 @@
       </c>
     </row>
     <row r="90" spans="1:9">
-      <c r="A90" s="17"/>
-      <c r="B90" s="17"/>
+      <c r="A90" s="18"/>
+      <c r="B90" s="18"/>
       <c r="D90" s="1" t="s">
         <v>11</v>
       </c>
@@ -3094,8 +3153,8 @@
       </c>
     </row>
     <row r="91" spans="1:9">
-      <c r="A91" s="17"/>
-      <c r="B91" s="17" t="s">
+      <c r="A91" s="18"/>
+      <c r="B91" s="18" t="s">
         <v>56</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -3118,8 +3177,8 @@
       </c>
     </row>
     <row r="92" spans="1:9">
-      <c r="A92" s="17"/>
-      <c r="B92" s="17"/>
+      <c r="A92" s="18"/>
+      <c r="B92" s="18"/>
       <c r="D92" s="1" t="s">
         <v>11</v>
       </c>
@@ -3140,8 +3199,8 @@
       </c>
     </row>
     <row r="93" spans="1:9">
-      <c r="A93" s="17"/>
-      <c r="B93" s="17" t="s">
+      <c r="A93" s="18"/>
+      <c r="B93" s="18" t="s">
         <v>57</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -3164,8 +3223,8 @@
       </c>
     </row>
     <row r="94" spans="1:9">
-      <c r="A94" s="17"/>
-      <c r="B94" s="17"/>
+      <c r="A94" s="18"/>
+      <c r="B94" s="18"/>
       <c r="D94" s="1" t="s">
         <v>11</v>
       </c>
@@ -3186,10 +3245,10 @@
       </c>
     </row>
     <row r="95" spans="1:9">
-      <c r="A95" s="14" t="s">
+      <c r="A95" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B95" s="14" t="s">
+      <c r="B95" s="15" t="s">
         <v>59</v>
       </c>
       <c r="C95" s="3"/>
@@ -3236,10 +3295,10 @@
       </c>
     </row>
     <row r="97" spans="1:9">
-      <c r="A97" s="17" t="s">
+      <c r="A97" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B97" s="17" t="s">
+      <c r="B97" s="18" t="s">
         <v>61</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -3262,8 +3321,8 @@
       </c>
     </row>
     <row r="98" spans="1:9">
-      <c r="A98" s="17"/>
-      <c r="B98" s="17"/>
+      <c r="A98" s="18"/>
+      <c r="B98" s="18"/>
       <c r="D98" s="1" t="s">
         <v>11</v>
       </c>
@@ -3284,10 +3343,10 @@
       </c>
     </row>
     <row r="99" spans="1:9">
-      <c r="A99" s="14" t="s">
+      <c r="A99" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B99" s="14" t="s">
+      <c r="B99" s="15" t="s">
         <v>63</v>
       </c>
       <c r="C99" s="3"/>
@@ -3334,10 +3393,10 @@
       </c>
     </row>
     <row r="101" spans="1:9">
-      <c r="A101" s="17" t="s">
+      <c r="A101" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B101" s="17" t="s">
+      <c r="B101" s="18" t="s">
         <v>65</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -3360,8 +3419,8 @@
       </c>
     </row>
     <row r="102" spans="1:9">
-      <c r="A102" s="17"/>
-      <c r="B102" s="17"/>
+      <c r="A102" s="18"/>
+      <c r="B102" s="18"/>
       <c r="D102" s="1" t="s">
         <v>11</v>
       </c>
@@ -3382,10 +3441,10 @@
       </c>
     </row>
     <row r="103" spans="1:9">
-      <c r="A103" s="14" t="s">
+      <c r="A103" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B103" s="14" t="s">
+      <c r="B103" s="15" t="s">
         <v>67</v>
       </c>
       <c r="C103" s="3"/>
@@ -3432,10 +3491,10 @@
       </c>
     </row>
     <row r="105" spans="1:9">
-      <c r="A105" s="17" t="s">
+      <c r="A105" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B105" s="17" t="s">
+      <c r="B105" s="18" t="s">
         <v>69</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -3458,8 +3517,8 @@
       </c>
     </row>
     <row r="106" spans="1:9">
-      <c r="A106" s="17"/>
-      <c r="B106" s="17"/>
+      <c r="A106" s="18"/>
+      <c r="B106" s="18"/>
       <c r="D106" s="1" t="s">
         <v>11</v>
       </c>
@@ -3480,8 +3539,8 @@
       </c>
     </row>
     <row r="107" spans="1:9">
-      <c r="A107" s="17"/>
-      <c r="B107" s="17" t="s">
+      <c r="A107" s="18"/>
+      <c r="B107" s="18" t="s">
         <v>70</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -3504,8 +3563,8 @@
       </c>
     </row>
     <row r="108" spans="1:9">
-      <c r="A108" s="17"/>
-      <c r="B108" s="17"/>
+      <c r="A108" s="18"/>
+      <c r="B108" s="18"/>
       <c r="D108" s="1" t="s">
         <v>11</v>
       </c>
@@ -3526,10 +3585,10 @@
       </c>
     </row>
     <row r="109" spans="1:9">
-      <c r="A109" s="14" t="s">
+      <c r="A109" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B109" s="14" t="s">
+      <c r="B109" s="15" t="s">
         <v>72</v>
       </c>
       <c r="C109" s="3"/>
@@ -3576,10 +3635,10 @@
       </c>
     </row>
     <row r="111" spans="1:9">
-      <c r="A111" s="17" t="s">
+      <c r="A111" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B111" s="17" t="s">
+      <c r="B111" s="18" t="s">
         <v>74</v>
       </c>
       <c r="D111" s="1" t="s">
@@ -3602,8 +3661,8 @@
       </c>
     </row>
     <row r="112" spans="1:9">
-      <c r="A112" s="17"/>
-      <c r="B112" s="17"/>
+      <c r="A112" s="18"/>
+      <c r="B112" s="18"/>
       <c r="D112" s="1" t="s">
         <v>11</v>
       </c>
@@ -3624,10 +3683,10 @@
       </c>
     </row>
     <row r="113" spans="1:9">
-      <c r="A113" s="14" t="s">
+      <c r="A113" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B113" s="14" t="s">
+      <c r="B113" s="15" t="s">
         <v>76</v>
       </c>
       <c r="C113" s="3"/>
@@ -3651,8 +3710,8 @@
       </c>
     </row>
     <row r="114" spans="1:9">
-      <c r="A114" s="15"/>
-      <c r="B114" s="15"/>
+      <c r="A114" s="17"/>
+      <c r="B114" s="17"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4" t="s">
         <v>11</v>
@@ -3674,8 +3733,8 @@
       </c>
     </row>
     <row r="115" spans="1:9">
-      <c r="A115" s="15"/>
-      <c r="B115" s="15" t="s">
+      <c r="A115" s="17"/>
+      <c r="B115" s="17" t="s">
         <v>77</v>
       </c>
       <c r="C115" s="4"/>
@@ -3722,10 +3781,10 @@
       </c>
     </row>
     <row r="117" spans="1:9">
-      <c r="A117" s="14" t="s">
+      <c r="A117" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B117" s="14" t="s">
+      <c r="B117" s="15" t="s">
         <v>79</v>
       </c>
       <c r="C117" s="3"/>
@@ -3749,8 +3808,8 @@
       </c>
     </row>
     <row r="118" spans="1:9">
-      <c r="A118" s="15"/>
-      <c r="B118" s="15"/>
+      <c r="A118" s="17"/>
+      <c r="B118" s="17"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4" t="s">
         <v>11</v>
@@ -3772,8 +3831,8 @@
       </c>
     </row>
     <row r="119" spans="1:9">
-      <c r="A119" s="15"/>
-      <c r="B119" s="15" t="s">
+      <c r="A119" s="17"/>
+      <c r="B119" s="17" t="s">
         <v>80</v>
       </c>
       <c r="C119" s="4"/>
@@ -3797,8 +3856,8 @@
       </c>
     </row>
     <row r="120" spans="1:9">
-      <c r="A120" s="15"/>
-      <c r="B120" s="15"/>
+      <c r="A120" s="17"/>
+      <c r="B120" s="17"/>
       <c r="C120" s="4"/>
       <c r="D120" s="4" t="s">
         <v>11</v>
@@ -3820,8 +3879,8 @@
       </c>
     </row>
     <row r="121" spans="1:9">
-      <c r="A121" s="15"/>
-      <c r="B121" s="15" t="s">
+      <c r="A121" s="17"/>
+      <c r="B121" s="17" t="s">
         <v>81</v>
       </c>
       <c r="C121" s="4"/>
@@ -3845,8 +3904,8 @@
       </c>
     </row>
     <row r="122" spans="1:9">
-      <c r="A122" s="15"/>
-      <c r="B122" s="15"/>
+      <c r="A122" s="17"/>
+      <c r="B122" s="17"/>
       <c r="C122" s="4"/>
       <c r="D122" s="4" t="s">
         <v>11</v>
@@ -3868,8 +3927,8 @@
       </c>
     </row>
     <row r="123" spans="1:9">
-      <c r="A123" s="15"/>
-      <c r="B123" s="15" t="s">
+      <c r="A123" s="17"/>
+      <c r="B123" s="17" t="s">
         <v>82</v>
       </c>
       <c r="C123" s="4"/>
@@ -3893,8 +3952,8 @@
       </c>
     </row>
     <row r="124" spans="1:9" ht="16" thickBot="1">
-      <c r="A124" s="18"/>
-      <c r="B124" s="18"/>
+      <c r="A124" s="22"/>
+      <c r="B124" s="22"/>
       <c r="C124" s="6"/>
       <c r="D124" s="6" t="s">
         <v>11</v>
@@ -3924,23 +3983,23 @@
       </c>
       <c r="E125" s="12">
         <f t="array" ref="E125">SUM((MOD(ROW(E3:E124)-ROW(E3),2)=0)*(E3:E124))/(0.5*COUNT(E3:E124))</f>
-        <v>64.805872727272742</v>
+        <v>61.453844827586224</v>
       </c>
       <c r="F125" s="12">
         <f t="array" ref="F125">SUM((MOD(ROW(F3:F124)-ROW(F3),2)=0)*(F3:F124))/(0.5*COUNT(F3:F124))</f>
-        <v>16.981818181818181</v>
+        <v>16.103448275862068</v>
       </c>
       <c r="G125" s="12">
         <f t="array" ref="G125">SUM((MOD(ROW(G3:G124)-ROW(G3),2)=0)*(G3:G124))/(0.5*COUNT(G3:G124))</f>
-        <v>3.0767272727272732</v>
+        <v>2.9175862068965523</v>
       </c>
       <c r="H125" s="12">
         <f t="array" ref="H125">SUM((MOD(ROW(H3:H124)-ROW(H3),2)=0)*(H3:H124))/(0.5*COUNT(H3:H124))</f>
-        <v>3.1487272727272715</v>
+        <v>2.985862068965516</v>
       </c>
       <c r="I125" s="12">
         <f t="array" ref="I125">SUM((MOD(ROW(I3:I124)-ROW(I3),2)=0)*(I3:I124))/(0.5*COUNT(I3:I124))</f>
-        <v>38.418181818181822</v>
+        <v>36.431034482758619</v>
       </c>
     </row>
     <row r="126" spans="1:9">
@@ -3952,23 +4011,23 @@
       </c>
       <c r="E126" s="13">
         <f t="array" ref="E126">SUM((MOD(ROW(E3:E124)-ROW(E3),2)=1)*(E3:E124))/(0.5*COUNT(E3:E124))</f>
-        <v>1.2127272727272729</v>
+        <v>1.2960344827586205</v>
       </c>
       <c r="F126" s="13">
         <f t="array" ref="F126">SUM((MOD(ROW(F3:F124)-ROW(F3),2)=1)*(F3:F124))/(0.5*COUNT(F3:F124))</f>
-        <v>86.890909090909091</v>
+        <v>92.58620689655173</v>
       </c>
       <c r="G126" s="13">
         <f t="array" ref="G126">SUM((MOD(ROW(G3:G124)-ROW(G3),2)=1)*(G3:G124))/(0.5*COUNT(G3:G124))</f>
-        <v>3.5994545454545452</v>
+        <v>4.1570689655172419</v>
       </c>
       <c r="H126" s="13">
         <f t="array" ref="H126">SUM((MOD(ROW(H3:H124)-ROW(H3),2)=1)*(H3:H124))/(0.5*COUNT(H3:H124))</f>
-        <v>1.5432727272727278</v>
+        <v>1.6658620689655175</v>
       </c>
       <c r="I126" s="13">
         <f t="array" ref="I126">SUM((MOD(ROW(I3:I124)-ROW(I3),2)=1)*(I3:I124))/(0.5*COUNT(I3:I124))</f>
-        <v>74.163636363636357</v>
+        <v>78.206896551724142</v>
       </c>
     </row>
     <row r="127" spans="1:9">
@@ -3982,38 +4041,54 @@
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="A101:A102"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B117:B118"/>
+    <mergeCell ref="B119:B120"/>
+    <mergeCell ref="B121:B122"/>
+    <mergeCell ref="B123:B124"/>
+    <mergeCell ref="B113:B114"/>
+    <mergeCell ref="B115:B116"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="A81:A84"/>
+    <mergeCell ref="A87:A88"/>
+    <mergeCell ref="A89:A94"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="A113:A116"/>
+    <mergeCell ref="A117:A124"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="B105:B106"/>
+    <mergeCell ref="B107:B108"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="B111:B112"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="B101:B102"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="A1:A2"/>
@@ -4038,54 +4113,38 @@
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B117:B118"/>
-    <mergeCell ref="B119:B120"/>
-    <mergeCell ref="B121:B122"/>
-    <mergeCell ref="B123:B124"/>
-    <mergeCell ref="B113:B114"/>
-    <mergeCell ref="B115:B116"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="A81:A84"/>
-    <mergeCell ref="A87:A88"/>
-    <mergeCell ref="A89:A94"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="A113:A116"/>
-    <mergeCell ref="A117:A124"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="B105:B106"/>
-    <mergeCell ref="B107:B108"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="B111:B112"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="B101:B102"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="A101:A102"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>